<commit_message>
learnt testng xml file direct runs
</commit_message>
<xml_diff>
--- a/DataFiles/VisitFranklinSite - Copy.xlsx
+++ b/DataFiles/VisitFranklinSite - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\eclipse-workspace\JavaTraining\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\New folder\Test\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE0871-CA39-47D5-8174-86AE4A5F9EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE806F9E-2D64-422B-8216-37F862444C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4D31ABB0-7AB1-4C97-B742-8AEAD6108B56}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Mobile</t>
   </si>
@@ -166,34 +166,43 @@
     <t>https://visitfranklin.tekark.com/blog/fun-for-the-whole-family-in-franklin-southampton-va/</t>
   </si>
   <si>
-    <t>https://www.dominionterminal.com/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/facility-operations/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/about-us/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/stewardship/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/employment/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/contact-us/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/employees/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/privacy-notice/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/disclaimer/</t>
-  </si>
-  <si>
-    <t>https://www.dominionterminal.com/terms-conditions/</t>
+    <t>https://unitedwayshr.org/staging/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/what-we-do/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/what-we-do/united-for-children/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/what-we-do/mission-united/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/what-we-do/developmental-screening/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/what-we-do/project-inclusion/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/get-involved/give/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/get-involved/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/about/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/about/events/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/about/our-team/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/give/</t>
+  </si>
+  <si>
+    <t>https://unitedwayshr.org/staging/toolkit/</t>
   </si>
 </sst>
 </file>
@@ -324,14 +333,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -648,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FFD22-1BC1-480C-8676-4E6D79DA8FDB}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,45 +679,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -842,22 +851,64 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{E8E26557-148D-4E93-88B0-60878DAB300F}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{7642F7F1-5634-4752-AFFD-3E8741E4E10D}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{8A9EF3FF-6727-4B9E-9EC4-1F12825C08CE}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{CA7669C5-09C1-4DDD-A21D-7783567DA5F6}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{18A0B2CA-817F-43AD-9354-D68CFE098F5E}"/>
-    <hyperlink ref="A8" r:id="rId6" xr:uid="{FFEC82B8-4653-42E7-BEBE-086ECE53F0E4}"/>
-    <hyperlink ref="A9" r:id="rId7" xr:uid="{9EFFE0AE-5716-478C-8B05-A9351D7500A8}"/>
-    <hyperlink ref="A10" r:id="rId8" xr:uid="{AC462931-1E61-4BD4-9EE3-84D2C0E51106}"/>
-    <hyperlink ref="A11" r:id="rId9" xr:uid="{D4C2DC60-3DB1-4A59-AF57-1BB9AA1F891C}"/>
-    <hyperlink ref="A12" r:id="rId10" xr:uid="{8C3D4E8E-8ECB-489E-BBBC-7E0B6D535C34}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{3E7C8D2C-1FF8-4A19-BBBF-0ACDB57A8DF4}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{C908A25C-37A8-47BE-AE44-D4CDBD70567C}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{6930315A-82AD-4061-850E-503DD5C02CE4}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{CCE6297D-52BE-460E-A44C-C71ED65B5EB3}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{EDC2EBC3-A88D-4B2A-AE9F-91EBA291BEC9}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{7681B2A8-F79C-462F-B0B1-C1797D4BB500}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{E6D232D0-FC42-4BD2-8079-AC28A8A153D3}"/>
+    <hyperlink ref="A10" r:id="rId8" display="https://unitedwayshr.org/staging/get-involved/give/" xr:uid="{1B2243F5-CF64-4D2A-8868-0C78690DD286}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{BFE94B6E-DBFB-4CE1-9BC2-266B9305E9EC}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{DAACB1C8-C7FC-4782-A223-8FFD05E5787C}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{EC845EC7-EA08-48FE-BB9E-535831F6A42D}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{1AF265CA-D35C-46F8-BF5B-2B0B0D804C8E}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{1E22D0D0-5D48-4F98-B760-6667514794B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>